<commit_message>
Bad nutrients recommendations fix. Analytics, new design.
</commit_message>
<xml_diff>
--- a/files/Translations.xlsx
+++ b/files/Translations.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="658">
   <si>
     <t>TranslateId</t>
   </si>
@@ -1954,6 +1954,42 @@
   </si>
   <si>
     <t>primeri jelovnika</t>
+  </si>
+  <si>
+    <t>meal</t>
+  </si>
+  <si>
+    <t>obrok</t>
+  </si>
+  <si>
+    <t>energy value</t>
+  </si>
+  <si>
+    <t>energetska vrijednost</t>
+  </si>
+  <si>
+    <t>energetska vrednost</t>
+  </si>
+  <si>
+    <t>recommended dietary allowance</t>
+  </si>
+  <si>
+    <t>preporućena dnevna količina</t>
+  </si>
+  <si>
+    <t>minimum dietary allowance</t>
+  </si>
+  <si>
+    <t>minimalna dnevna potreba</t>
+  </si>
+  <si>
+    <t>upper intake level</t>
+  </si>
+  <si>
+    <t>najveći prihvatljiv dnevni unos</t>
+  </si>
+  <si>
+    <t>ul</t>
   </si>
 </sst>
 </file>
@@ -2300,8 +2336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:Q390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A301" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B308" sqref="B308"/>
+    <sheetView tabSelected="1" topLeftCell="A303" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D314" sqref="D314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8204,10 +8240,10 @@
         <v>totals</v>
       </c>
       <c r="D221" s="4" t="s">
-        <v>123</v>
+        <v>394</v>
       </c>
       <c r="E221" t="s">
-        <v>123</v>
+        <v>578</v>
       </c>
       <c r="I221" t="str">
         <f t="shared" si="14"/>
@@ -8215,11 +8251,11 @@
       </c>
       <c r="L221" t="str">
         <f t="shared" si="15"/>
-        <v>'totals':'ukupno',</v>
+        <v>'totals':'ukupne vrijednosti',</v>
       </c>
       <c r="O221" t="str">
         <f t="shared" si="16"/>
-        <v>'totals':'ukupno',</v>
+        <v>'totals':'ukupne vrednosti',</v>
       </c>
     </row>
     <row r="222" spans="2:15">
@@ -10532,135 +10568,170 @@
       </c>
     </row>
     <row r="308" spans="2:15">
-      <c r="C308" s="4">
+      <c r="B308" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="C308" s="4" t="str">
         <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="E308">
+        <v>meal</v>
+      </c>
+      <c r="D308" s="4" t="s">
+        <v>647</v>
+      </c>
+      <c r="E308" t="str">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>obrok</v>
       </c>
       <c r="I308" t="str">
         <f t="shared" si="18"/>
-        <v>'':'0',</v>
+        <v>'meal':'meal',</v>
       </c>
       <c r="L308" t="str">
         <f t="shared" si="19"/>
-        <v>'':'',</v>
+        <v>'meal':'obrok',</v>
       </c>
       <c r="O308" t="str">
         <f t="shared" si="20"/>
-        <v>'':'0',</v>
+        <v>'meal':'obrok',</v>
       </c>
     </row>
     <row r="309" spans="2:15">
-      <c r="C309" s="4">
+      <c r="B309" s="4" t="s">
+        <v>648</v>
+      </c>
+      <c r="C309" s="4" t="str">
         <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="E309">
-        <f t="shared" si="22"/>
-        <v>0</v>
+        <v>energy value</v>
+      </c>
+      <c r="D309" s="4" t="s">
+        <v>649</v>
+      </c>
+      <c r="E309" t="s">
+        <v>650</v>
       </c>
       <c r="I309" t="str">
         <f t="shared" si="18"/>
-        <v>'':'0',</v>
+        <v>'energy value':'energy value',</v>
       </c>
       <c r="L309" t="str">
         <f t="shared" si="19"/>
-        <v>'':'',</v>
+        <v>'energy value':'energetska vrijednost',</v>
       </c>
       <c r="O309" t="str">
         <f t="shared" si="20"/>
-        <v>'':'0',</v>
+        <v>'energy value':'energetska vrednost',</v>
       </c>
     </row>
     <row r="310" spans="2:15">
-      <c r="C310" s="4">
+      <c r="B310" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="C310" s="4" t="str">
         <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="E310">
+        <v>recommended dietary allowance</v>
+      </c>
+      <c r="D310" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="E310" t="str">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>preporućena dnevna količina</v>
       </c>
       <c r="I310" t="str">
         <f t="shared" si="18"/>
-        <v>'':'0',</v>
+        <v>'recommended dietary allowance':'recommended dietary allowance',</v>
       </c>
       <c r="L310" t="str">
         <f t="shared" si="19"/>
-        <v>'':'',</v>
+        <v>'recommended dietary allowance':'preporućena dnevna količina',</v>
       </c>
       <c r="O310" t="str">
         <f t="shared" si="20"/>
-        <v>'':'0',</v>
+        <v>'recommended dietary allowance':'preporućena dnevna količina',</v>
       </c>
     </row>
     <row r="311" spans="2:15">
-      <c r="C311" s="4">
+      <c r="B311" s="4" t="s">
+        <v>653</v>
+      </c>
+      <c r="C311" s="4" t="str">
         <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="E311">
+        <v>minimum dietary allowance</v>
+      </c>
+      <c r="D311" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="E311" t="str">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>minimalna dnevna potreba</v>
       </c>
       <c r="I311" t="str">
         <f t="shared" si="18"/>
-        <v>'':'0',</v>
+        <v>'minimum dietary allowance':'minimum dietary allowance',</v>
       </c>
       <c r="L311" t="str">
         <f t="shared" si="19"/>
-        <v>'':'',</v>
+        <v>'minimum dietary allowance':'minimalna dnevna potreba',</v>
       </c>
       <c r="O311" t="str">
         <f t="shared" si="20"/>
-        <v>'':'0',</v>
+        <v>'minimum dietary allowance':'minimalna dnevna potreba',</v>
       </c>
     </row>
     <row r="312" spans="2:15">
-      <c r="C312" s="4">
+      <c r="B312" s="4" t="s">
+        <v>655</v>
+      </c>
+      <c r="C312" s="4" t="str">
         <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="E312">
+        <v>upper intake level</v>
+      </c>
+      <c r="D312" s="4" t="s">
+        <v>656</v>
+      </c>
+      <c r="E312" t="str">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>najveći prihvatljiv dnevni unos</v>
       </c>
       <c r="I312" t="str">
         <f t="shared" si="18"/>
-        <v>'':'0',</v>
+        <v>'upper intake level':'upper intake level',</v>
       </c>
       <c r="L312" t="str">
         <f t="shared" si="19"/>
-        <v>'':'',</v>
+        <v>'upper intake level':'najveći prihvatljiv dnevni unos',</v>
       </c>
       <c r="O312" t="str">
         <f t="shared" si="20"/>
-        <v>'':'0',</v>
+        <v>'upper intake level':'najveći prihvatljiv dnevni unos',</v>
       </c>
     </row>
     <row r="313" spans="2:15">
-      <c r="C313" s="4">
+      <c r="B313" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="C313" s="4" t="str">
         <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="E313">
+        <v>ul</v>
+      </c>
+      <c r="D313" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="E313" t="str">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>ul</v>
       </c>
       <c r="I313" t="str">
         <f t="shared" si="18"/>
-        <v>'':'0',</v>
+        <v>'ul':'ul',</v>
       </c>
       <c r="L313" t="str">
         <f t="shared" si="19"/>
-        <v>'':'',</v>
+        <v>'ul':'ul',</v>
       </c>
       <c r="O313" t="str">
         <f t="shared" si="20"/>
-        <v>'':'0',</v>
+        <v>'ul':'ul',</v>
       </c>
     </row>
     <row r="314" spans="2:15">

</xml_diff>